<commit_message>
j'ai enfilé la soubrette, c'est tout propre hihi
</commit_message>
<xml_diff>
--- a/res/Classeur1.xlsx
+++ b/res/Classeur1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Desktop\IUT\s202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Desktop\IUT\s202\A-G5\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235AB6BB-155E-43D6-90B4-2D6CDF025386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4027DA-8E79-4D32-88D3-395C360C5591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13245" yWindow="4950" windowWidth="21600" windowHeight="11835" xr2:uid="{E1C18CE6-A35D-4F59-9FEC-44D04BCDD4A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1C18CE6-A35D-4F59-9FEC-44D04BCDD4A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E329265-AF2B-4F21-81B7-2C9FB652761D}">
   <dimension ref="B2:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K43" workbookViewId="0">
-      <selection activeCell="S62" sqref="S62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,10 +1222,10 @@
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>13</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>AVERAGE(C18:C24)</f>
         <v>9.9857142857142858</v>
@@ -1530,7 +1530,7 @@
       <c r="K25" s="21"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O26" s="20" t="s">
         <v>19</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O27" s="18" t="s">
         <v>11</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>2.3330519227722424</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O28" s="18" t="s">
         <v>12</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>2.6988747834239062</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O29" s="18" t="s">
         <v>13</v>
       </c>
@@ -1621,8 +1621,12 @@
       <c r="U29" s="12">
         <v>2.6460880346138436</v>
       </c>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="1">
+        <f>U31+Q29+R27+T30+S28+P32</f>
+        <v>11.941083725111488</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O30" s="18" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>2.130947092623972</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O31" s="18" t="s">
         <v>16</v>
       </c>
@@ -1668,7 +1672,7 @@
         <v>2.4547257425147317</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="O32" s="19" t="s">
         <v>17</v>
       </c>

</xml_diff>